<commit_message>
Added Vlookup formula Sheet
</commit_message>
<xml_diff>
--- a/Week/RequiredFiles/FormulaSheet.xlsx
+++ b/Week/RequiredFiles/FormulaSheet.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FormulaSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="System Path" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -399,16 +400,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="23.6328125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="142.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="23.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="103.44140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="31" customWidth="1" min="3" max="3"/>
+    <col width="14.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="17.5546875" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">
@@ -419,7 +423,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Formula</t>
+          <t>Formula Path</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>VLOOKUP Formula</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Input File Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
         </is>
       </c>
     </row>
@@ -431,7 +455,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VLOOKUP(Val5,'C:\C-BIA\PurchaseOrder\Week\RequiredFiles\[Location Master.xlsx]Location Master'!$A$2:$B$22,2,FALSE)</t>
+          <t>VLOOKUP(#VAL#5,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Location Master.xlsx]Location Master'!$A$2:$B$22,2,FALSE)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>VLOOKUP(#VAL#5,'{PATH}[Location Master.xlsx]Location Master'!$A$2:$B$22,2,FALSE)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Location Master</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pivot/Requ Sum</t>
         </is>
       </c>
     </row>
@@ -443,7 +482,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VLOOKUP(BVal,'C:\C-BIA\PurchaseOrder\Week\RequiredFiles\[Item Master.xlsx]Item Master'!$O$2:$W$22287,3,FALSE)</t>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Item Master.xlsx]Item Master'!$A:$S,19,FALSE)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Item Master.xlsx]Item Master'!$A:$S,19,FALSE)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Item Master</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
         </is>
       </c>
     </row>
@@ -453,6 +507,26 @@
           <t>Style</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Item Master.xlsx]Item Master'!$A:$C,3,FALSE)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Item Master.xlsx]Item Master'!$A:$C,3,FALSE)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Item Master</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -462,7 +536,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLOOKUP(BVal,'C:\C-BIA\PurchaseOrder\Week\RequiredFiles\[Item Master.xlsx]Item Master'!$O$2:$W$22287,8,FALSE)</t>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Item Master.xlsx]Item Master'!$A:$B,2,FALSE)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Item Master.xlsx]Item Master'!$A:$B,2,FALSE)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Item Master</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
         </is>
       </c>
     </row>
@@ -472,6 +561,26 @@
           <t>Rate</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Item Master.xlsx]Item Master'!$A:$M,13,FALSE)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Item Master.xlsx]Item Master'!$A:$M,13,FALSE)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Item Master</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -479,6 +588,21 @@
           <t>Location 2</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Location 2 Master.xlsx]Sheet1'!$A:$C,3,FALSE)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Location 2 Master.xlsx]Sheet1'!$A:$C,3,FALSE)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -486,6 +610,21 @@
           <t>BULK/DTA BULK/ EOSS LOC</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Location 2 Master.xlsx]Sheet1'!$A:$D,4,FALSE)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Location 2 Master.xlsx]Sheet1'!$A:$D,4,FALSE)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -493,16 +632,88 @@
           <t>MRP</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[Item Master.xlsx]Item Master'!$A:$M,13,FALSE)</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>VLOOKUP(B#VAL#,'{PATH}[Item Master.xlsx]Item Master'!$A:$M,13,FALSE)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Item Master</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Closing Stock</t>
+          <t>Closing Stock - PIVOT</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>VLOOKUP(A#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\Master Files\[WH Closing Stock.xlsx]TII STK MBO KAM'!$A:$V,22,FALSE)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>VLOOKUP(A#VAL#,'{PATH}[WH Closing Stock.xlsx]TII STK MBO KAM'!$A:$V,22,FALSE)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>WH Closing Stock</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pivot/Requ Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Closing Stock - Template</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Pivot/Requ Sum</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Packaking Template</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>In Different Folder</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>In Different Folder</t>
         </is>
       </c>
     </row>
@@ -510,4 +721,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>C:\Users\HP\Desktop\TrimphPO\Week\Master Files\</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in floder structure added logs and put functions to main.py file
</commit_message>
<xml_diff>
--- a/Week/RequiredFiles/FormulaSheet.xlsx
+++ b/Week/RequiredFiles/FormulaSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="FormulaSheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -456,10 +456,10 @@
   </sheetPr>
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A21" sqref="A21"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -744,12 +744,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>VLOOKUP(B#VAL#,'C:\C-BIA\PurchaseOrder\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>VLOOKUP(B#VAL#,'C:\C-BIA\PurchaseOrder\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
+          <t>VLOOKUP(B#VAL#,'C:\Users\HP\Desktop\TrimphPO\Week\PivotTable\[PivotTableoutput.xlsx]Sheet1'!$A:$X,24,FALSE)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1520,8 +1520,8 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>